<commit_message>
add keys and reformat melatonin tables
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -140,7 +140,9 @@
 Prodrome frequency tables</t>
   </si>
   <si>
-    <t>Melatonin random-contolled n's &amp; %'s -placebo AEs</t>
+    <t>Melatonin random-contolled n's &amp; %'s -placebo AEs
+Corrections and additions to melatonin data
+Melatonin efficacy data</t>
   </si>
 </sst>
 </file>
@@ -964,7 +966,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="34"/>
     </row>
-    <row r="13" spans="2:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" s="33" customFormat="1" ht="57" x14ac:dyDescent="0.25">
       <c r="B13" s="39">
         <v>42899</v>
       </c>
@@ -975,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="41">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="34"/>
@@ -994,7 +996,7 @@
       </c>
       <c r="E15" s="46">
         <f>SUM(E5:E14)</f>
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="20" thickTop="1" x14ac:dyDescent="0.25">
@@ -1003,7 +1005,7 @@
       </c>
       <c r="E16" s="14">
         <f>(SUM(G:G) - E15*10)</f>
-        <v>-70</v>
+        <v>-140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to Melatonin AE frequency summary
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Work carried out for Prof Besag</t>
   </si>
@@ -85,6 +85,19 @@
     <t>Summary of prodrome EEG algorithm performance
 Summary of prodrome incidences (%)
 Summary of melatonin adverse effects incidences (%)</t>
+  </si>
+  <si>
+    <t>Updates to melatonin summary
+Melatonin frequency tables
+Prodrome frequency tables</t>
+  </si>
+  <si>
+    <t>Melatonin random-contolled n's &amp; %'s -placebo AEs
+Corrections and additions to melatonin data
+Melatonin efficacy data</t>
+  </si>
+  <si>
+    <t>Melatonin efficacy data completed (available pdfs)</t>
   </si>
   <si>
     <r>
@@ -100,10 +113,10 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="8" tint="-0.499984740745262"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>/</t>
+      <t>|</t>
     </r>
     <r>
       <rPr>
@@ -135,21 +148,49 @@
     </r>
   </si>
   <si>
-    <t>Updates to melatonin summary
-Melatonin frequency tables
-Prodrome frequency tables</t>
-  </si>
-  <si>
-    <t>Melatonin random-contolled n's &amp; %'s -placebo AEs
-Corrections and additions to melatonin data
-Melatonin efficacy data</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CREDIT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">DEBIT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>hrs</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,6 +268,12 @@
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -242,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -339,11 +386,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4" tint="0.59996337778862885"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -474,11 +530,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -486,6 +564,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -778,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -958,7 +1106,7 @@
         <v>42898</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="29">
         <v>12</v>
@@ -974,7 +1122,7 @@
         <v>42906</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="41">
         <v>15</v>
@@ -982,39 +1130,91 @@
       <c r="F13" s="42"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:7" s="47" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45" t="s">
+    <row r="14" spans="2:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="39">
+        <v>42907</v>
+      </c>
+      <c r="C14" s="39">
+        <v>42914</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="41">
+        <v>9</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:7" s="47" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="46">
-        <f>SUM(E5:E14)</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="14">
-        <f>(SUM(G:G) - E15*10)</f>
-        <v>-140</v>
+      <c r="E16" s="46">
+        <f>SUM(E5:E15)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="50" t="str">
+        <f>"PAID HOURS @ £10/hr = " &amp; SUM(G:G)  &amp; "/10"</f>
+        <v>PAID HOURS @ £10/hr = 1000/10</v>
+      </c>
+      <c r="E17" s="51">
+        <f>SUM(G:G)/10</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="47" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="48">
+        <f>E17-E16</f>
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="20" spans="2:5" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="14">
+        <f>(SUM(G:G) - E16*10)</f>
+        <v>-230</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add old projects directory. Directory includes VBA Initial Assessment files
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -95,9 +95,6 @@
     <t>Melatonin random-contolled n's &amp; %'s -placebo AEs
 Corrections and additions to melatonin data
 Melatonin efficacy data</t>
-  </si>
-  <si>
-    <t>Melatonin efficacy data completed (available pdfs)</t>
   </si>
   <si>
     <r>
@@ -184,6 +181,11 @@
       </rPr>
       <t>hrs</t>
     </r>
+  </si>
+  <si>
+    <t>Melatonin efficacy data completed (available pdfs)
+Updated and extended melatonin AE data (available pdfs)
+EEG prodrome time-to-seizure data investigation</t>
   </si>
 </sst>
 </file>
@@ -399,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -542,11 +544,14 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -574,66 +579,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -928,7 +873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1130,18 +1077,18 @@
       <c r="F13" s="42"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="2:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" s="33" customFormat="1" ht="76" x14ac:dyDescent="0.25">
       <c r="B14" s="39">
         <v>42907</v>
       </c>
       <c r="C14" s="39">
         <v>42914</v>
       </c>
-      <c r="D14" s="40" t="s">
-        <v>17</v>
+      <c r="D14" s="52" t="s">
+        <v>19</v>
       </c>
       <c r="E14" s="41">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F14" s="42"/>
       <c r="G14" s="34"/>
@@ -1160,7 +1107,7 @@
       </c>
       <c r="E16" s="46">
         <f>SUM(E5:E15)</f>
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1179,11 +1126,11 @@
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="48">
         <f>E17-E16</f>
-        <v>-23</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="19" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,11 +1140,11 @@
     </row>
     <row r="20" spans="2:5" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D20" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="14">
         <f>(SUM(G:G) - E16*10)</f>
-        <v>-230</v>
+        <v>-290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update melatonin data from PDFs accessed 24/06
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Work carried out for Prof Besag</t>
   </si>
@@ -186,6 +186,11 @@
     <t>Melatonin efficacy data completed (available pdfs)
 Updated and extended melatonin AE data (available pdfs)
 EEG prodrome time-to-seizure data investigation</t>
+  </si>
+  <si>
+    <t>Data extracted from new melatonin pdfs
+Split melatonin AE table: &gt; 100 patients | &gt; 3 mths
+Data extracted from new prodrome pdfs</t>
   </si>
 </sst>
 </file>
@@ -871,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G20"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1055,7 @@
         <v>42891</v>
       </c>
       <c r="C12" s="27">
-        <v>42898</v>
+        <v>42897</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>15</v>
@@ -1063,10 +1068,10 @@
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="57" x14ac:dyDescent="0.25">
       <c r="B13" s="39">
-        <v>42899</v>
+        <v>42898</v>
       </c>
       <c r="C13" s="39">
-        <v>42906</v>
+        <v>42904</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>16</v>
@@ -1079,10 +1084,10 @@
     </row>
     <row r="14" spans="2:7" s="33" customFormat="1" ht="76" x14ac:dyDescent="0.25">
       <c r="B14" s="39">
-        <v>42907</v>
+        <v>42905</v>
       </c>
       <c r="C14" s="39">
-        <v>42914</v>
+        <v>42911</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>19</v>
@@ -1093,62 +1098,77 @@
       <c r="F14" s="42"/>
       <c r="G14" s="34"/>
     </row>
-    <row r="15" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:7" s="47" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="46">
-        <f>SUM(E5:E15)</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="57" x14ac:dyDescent="0.25">
+      <c r="B15" s="39">
+        <v>42912</v>
+      </c>
+      <c r="C15" s="39">
+        <v>42918</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="41">
+        <v>4</v>
+      </c>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="2:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" s="47" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
-      <c r="D17" s="50" t="str">
+      <c r="D17" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="46">
+        <f>SUM(E5:E15)</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="50" t="str">
         <f>"PAID HOURS @ £10/hr = " &amp; SUM(G:G)  &amp; "/10"</f>
         <v>PAID HOURS @ £10/hr = 1000/10</v>
       </c>
-      <c r="E17" s="51">
+      <c r="E18" s="51">
         <f>SUM(G:G)/10</f>
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="47" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="48">
-        <f>E17-E16</f>
-        <v>-29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" s="47" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
-      <c r="D19" s="49"/>
-    </row>
-    <row r="20" spans="2:5" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="D19" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="48">
+        <f>E18-E17</f>
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="49"/>
+    </row>
+    <row r="21" spans="2:5" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="14">
-        <f>(SUM(G:G) - E16*10)</f>
-        <v>-290</v>
+      <c r="E21" s="14">
+        <f>(SUM(G:G) - E17*10)</f>
+        <v>-330</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E20">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -1156,7 +1176,7 @@
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="E19">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update and advance melatonin sleep efficiency and summary data
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -190,7 +190,8 @@
   <si>
     <t>Data extracted from new melatonin pdfs
 Split melatonin AE table: &gt; 100 patients | &gt; 3 mths
-Data extracted from new prodrome pdfs</t>
+Data extracted from new prodrome pdfs
+Remove duplicate references from EndNote library</t>
   </si>
 </sst>
 </file>
@@ -878,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1098,7 +1099,7 @@
       <c r="F14" s="42"/>
       <c r="G14" s="34"/>
     </row>
-    <row r="15" spans="2:7" ht="57" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="76" x14ac:dyDescent="0.25">
       <c r="B15" s="39">
         <v>42912</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="41">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F15" s="42"/>
     </row>
@@ -1127,7 +1128,7 @@
       </c>
       <c r="E17" s="46">
         <f>SUM(E5:E15)</f>
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1151,7 @@
       </c>
       <c r="E19" s="48">
         <f>E18-E17</f>
-        <v>-33</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="20" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1164,7 +1165,7 @@
       </c>
       <c r="E21" s="14">
         <f>(SUM(G:G) - E17*10)</f>
-        <v>-330</v>
+        <v>-400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all melatonin tables with latest additional citations @ 01/07
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -879,9 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1110,7 +1108,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="41">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F15" s="42"/>
     </row>
@@ -1128,7 +1126,7 @@
       </c>
       <c r="E17" s="46">
         <f>SUM(E5:E15)</f>
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1151,7 +1149,7 @@
       </c>
       <c r="E19" s="48">
         <f>E18-E17</f>
-        <v>-40</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="20" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1165,7 +1163,7 @@
       </c>
       <c r="E21" s="14">
         <f>(SUM(G:G) - E17*10)</f>
-        <v>-400</v>
+        <v>-480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split melatonin worksheets: MLT; PLB; ALL
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -1108,7 +1108,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="41">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F15" s="42"/>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="E17" s="46">
         <f>SUM(E5:E15)</f>
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="E19" s="48">
         <f>E18-E17</f>
-        <v>-48</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="20" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="E21" s="14">
         <f>(SUM(G:G) - E17*10)</f>
-        <v>-480</v>
+        <v>-510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish first pass update of clinical prodrome papers
</commit_message>
<xml_diff>
--- a/Timesheet/work.xlsx
+++ b/Timesheet/work.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvasey/Desktop/Besag/Timesheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvasey/Dropbox/Besag/Timesheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -194,7 +194,8 @@
 Remove duplicate references from EndNote library</t>
   </si>
   <si>
-    <t>Data extracted from new prodrome pdfs</t>
+    <t>Data extracted from new prodrome pdfs
+Extend clinical prodrome data</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1116,7 @@
       </c>
       <c r="F15" s="42"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="38" x14ac:dyDescent="0.25">
       <c r="B16" s="39">
         <v>42919</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="41">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F16" s="42"/>
     </row>
@@ -1144,7 +1145,7 @@
       </c>
       <c r="E18" s="46">
         <f>SUM(E5:E16)</f>
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="2:5" s="47" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1168,7 @@
       </c>
       <c r="E20" s="48">
         <f>E19-E18</f>
-        <v>-56</v>
+        <v>-64</v>
       </c>
     </row>
     <row r="21" spans="2:5" s="47" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1181,7 +1182,7 @@
       </c>
       <c r="E22" s="14">
         <f>(SUM(G:G) - E18*10)</f>
-        <v>-560</v>
+        <v>-640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>